<commit_message>
[02/16] Excel2Json 시스템 제작
</commit_message>
<xml_diff>
--- a/Assets/Tables/Excel/CategoryTab.xlsx
+++ b/Assets/Tables/Excel/CategoryTab.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="시트1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sword</t>
   </si>
   <si>
     <t xml:space="preserve">sword_unselect</t>
@@ -178,16 +181,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,123 +384,126 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>10001001</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>10001002</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>10001003</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>10001004</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>10001005</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>10001006</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[02/21] CategoryTab 테이블 수정
</commit_message>
<xml_diff>
--- a/Assets/Tables/Excel/CategoryTab.xlsx
+++ b/Assets/Tables/Excel/CategoryTab.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">tab_name</t>
+    <t xml:space="preserve">type</t>
   </si>
   <si>
     <t xml:space="preserve">normal_sprite</t>
@@ -34,10 +34,19 @@
     <t xml:space="preserve">select_sprite</t>
   </si>
   <si>
+    <t xml:space="preserve">order</t>
+  </si>
+  <si>
     <t xml:space="preserve">long</t>
   </si>
   <si>
+    <t xml:space="preserve">Enum&lt;ItemType&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
   </si>
   <si>
     <t xml:space="preserve">sword</t>
@@ -181,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -194,7 +203,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,15 +398,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.72"/>
   </cols>
@@ -407,19 +424,25 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,13 +450,16 @@
         <v>10001001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,13 +467,16 @@
         <v>10001002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,13 +484,16 @@
         <v>10001003</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,13 +501,16 @@
         <v>10001004</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,13 +518,16 @@
         <v>10001005</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,13 +535,16 @@
         <v>10001006</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>